<commit_message>
Add Spreadsheet for Gameweek 4
</commit_message>
<xml_diff>
--- a/WHUPUP.xlsx
+++ b/WHUPUP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\OneDrive\Desktop\F_Football\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B5AED2-3663-496D-8286-08D3BB2079E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77EF7822-7834-454B-A731-D482697C6BD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-60" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{99B477C4-CCE4-43A8-837E-CF46EFFB0705}"/>
+    <workbookView xWindow="22932" yWindow="-60" windowWidth="23256" windowHeight="12576" xr2:uid="{99B477C4-CCE4-43A8-837E-CF46EFFB0705}"/>
   </bookViews>
   <sheets>
     <sheet name="Weekly Points" sheetId="1" r:id="rId1"/>
@@ -605,11 +605,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDD6DB57-DBEF-439C-86C8-55613737F70F}">
   <dimension ref="A1:F121"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B100" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B97" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F106" sqref="F92:F106"/>
+      <selection pane="bottomRight" activeCell="F107" sqref="F107:F121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2794,7 +2794,7 @@
         <v>10</v>
       </c>
       <c r="F109">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
@@ -3046,7 +3046,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4E08F3E-397A-4BD7-9E39-8A74D5B0AA3B}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -3183,7 +3183,7 @@
       </c>
       <c r="C11">
         <f>SUM('Weekly Points'!F107:F121)+C9</f>
-        <v>208</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change Table to show Latest Week at top & Change Font
</commit_message>
<xml_diff>
--- a/WHUPUP.xlsx
+++ b/WHUPUP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\OneDrive\Desktop\F_Football\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73CAFE5C-A4D6-45D9-9C40-A1F1F4F477CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8718E07A-2103-4BC0-A1F3-CDA54E6976AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{99B477C4-CCE4-43A8-837E-CF46EFFB0705}"/>
   </bookViews>
@@ -267,9 +267,6 @@
     <t>Wellbeck</t>
   </si>
   <si>
-    <t>N . Jackson</t>
-  </si>
-  <si>
     <t>Konate</t>
   </si>
   <si>
@@ -277,6 +274,9 @@
   </si>
   <si>
     <t>Everton</t>
+  </si>
+  <si>
+    <t>N. Jackson</t>
   </si>
 </sst>
 </file>
@@ -654,7 +654,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomRight" activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -850,10 +850,10 @@
         <v>6</v>
       </c>
       <c r="C10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D10" t="s">
         <v>78</v>
-      </c>
-      <c r="D10" t="s">
-        <v>79</v>
       </c>
       <c r="E10" t="s">
         <v>11</v>
@@ -970,7 +970,7 @@
         <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D16" t="s">
         <v>52</v>
@@ -1050,7 +1050,7 @@
         <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D20" t="s">
         <v>54</v>
@@ -1570,7 +1570,7 @@
         <v>6</v>
       </c>
       <c r="C46" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D46" t="s">
         <v>52</v>

</xml_diff>

<commit_message>
Redone Week 9 Update
</commit_message>
<xml_diff>
--- a/WHUPUP.xlsx
+++ b/WHUPUP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\OneDrive\Desktop\F_Football\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1516EB50-E08C-462F-812E-359AAE684B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A5B809-2AAE-4574-AA0A-77764A4077EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-60" windowWidth="23256" windowHeight="12576" xr2:uid="{99B477C4-CCE4-43A8-837E-CF46EFFB0705}"/>
+    <workbookView xWindow="22932" yWindow="-60" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{99B477C4-CCE4-43A8-837E-CF46EFFB0705}"/>
   </bookViews>
   <sheets>
     <sheet name="Weekly Points" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1109" uniqueCount="81">
   <si>
     <t>Gameweek</t>
   </si>
@@ -653,11 +653,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDD6DB57-DBEF-439C-86C8-55613737F70F}">
   <dimension ref="A1:F271"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomRight" activeCell="F17" sqref="F17:F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6095,10 +6095,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4E08F3E-397A-4BD7-9E39-8A74D5B0AA3B}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6333,10 +6333,34 @@
         <v>376</v>
       </c>
     </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <f>SUM('Weekly Points'!F242:F256)+C18</f>
+        <v>506</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21">
+        <v>9</v>
+      </c>
+      <c r="C21">
+        <f>SUM('Weekly Points'!F257:F271)+C19</f>
+        <v>439</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="C4:C5 C6 C7:C11 C12:C17 C18:C19" formulaRange="1"/>
+    <ignoredError sqref="C4:C5 C6 C7:C11 C12:C17 C18:C19 C20:C21" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cumulative Points Table updated
</commit_message>
<xml_diff>
--- a/WHUPUP.xlsx
+++ b/WHUPUP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\OneDrive\Desktop\F_Football\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A5B809-2AAE-4574-AA0A-77764A4077EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD7CAF7-B2C3-4B9C-B3D4-BD0CD0E6ED90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-60" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{99B477C4-CCE4-43A8-837E-CF46EFFB0705}"/>
   </bookViews>
@@ -654,10 +654,10 @@
   <dimension ref="A1:F271"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B244" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F17" sqref="F17:F31"/>
+      <selection pane="bottomRight" activeCell="F271" sqref="F1:F271"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6098,7 +6098,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6149,8 +6149,8 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <f>SUM('Weekly Points'!F2:F16)</f>
-        <v>50</v>
+        <f>SUMIFS('Weekly Points'!$F$2:$F$271,'Weekly Points'!$B$2:$B$271,"Bazzers Ballers",'Weekly Points'!$A$2:$A$271,B4)</f>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -6161,8 +6161,8 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <f>SUM('Weekly Points'!F17:F31)</f>
-        <v>47</v>
+        <f>SUMIFS('Weekly Points'!$F$2:$F$271,'Weekly Points'!$B$2:$B$271,"WHU-Tang-Clan",'Weekly Points'!$A$2:$A$271,B5)</f>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -6173,8 +6173,8 @@
         <v>2</v>
       </c>
       <c r="C6">
-        <f>SUM('Weekly Points'!F32:F46)+C4</f>
-        <v>78</v>
+        <f>SUMIFS('Weekly Points'!$F$2:$F$271,'Weekly Points'!$B$2:$B$271,"Bazzers Ballers",'Weekly Points'!$A$2:$A$271,B6)+C4</f>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -6185,8 +6185,8 @@
         <v>2</v>
       </c>
       <c r="C7">
-        <f>SUM('Weekly Points'!F47:F61)+C5</f>
-        <v>72</v>
+        <f>SUMIFS('Weekly Points'!$F$2:$F$271,'Weekly Points'!$B$2:$B$271,"WHU-Tang-Clan",'Weekly Points'!$A$2:$A$271,B7)+C5</f>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -6197,8 +6197,8 @@
         <v>3</v>
       </c>
       <c r="C8">
-        <f>SUM('Weekly Points'!F62:F76)+C6</f>
-        <v>114</v>
+        <f>SUMIFS('Weekly Points'!$F$2:$F$271,'Weekly Points'!$B$2:$B$271,"Bazzers Ballers",'Weekly Points'!$A$2:$A$271,B8)+C6</f>
+        <v>185</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -6209,8 +6209,8 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <f>SUM('Weekly Points'!F77:F91)+C7</f>
-        <v>120</v>
+        <f>SUMIFS('Weekly Points'!$F$2:$F$271,'Weekly Points'!$B$2:$B$271,"WHU-Tang-Clan",'Weekly Points'!$A$2:$A$271,B9)+C7</f>
+        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -6221,8 +6221,8 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <f>SUM('Weekly Points'!F92:F106)+C8</f>
-        <v>181</v>
+        <f>SUMIFS('Weekly Points'!$F$2:$F$271,'Weekly Points'!$B$2:$B$271,"Bazzers Ballers",'Weekly Points'!$A$2:$A$271,B10)+C8</f>
+        <v>262</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -6233,8 +6233,8 @@
         <v>4</v>
       </c>
       <c r="C11">
-        <f>SUM('Weekly Points'!F107:F121)+C9</f>
-        <v>172</v>
+        <f>SUMIFS('Weekly Points'!$F$2:$F$271,'Weekly Points'!$B$2:$B$271,"WHU-Tang-Clan",'Weekly Points'!$A$2:$A$271,B11)+C9</f>
+        <v>211</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -6245,8 +6245,8 @@
         <v>5</v>
       </c>
       <c r="C12">
-        <f>SUM('Weekly Points'!F122:F136)+C10</f>
-        <v>244</v>
+        <f>SUMIFS('Weekly Points'!$F$2:$F$271,'Weekly Points'!$B$2:$B$271,"Bazzers Ballers",'Weekly Points'!$A$2:$A$271,B12)+C10</f>
+        <v>325</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -6257,8 +6257,8 @@
         <v>5</v>
       </c>
       <c r="C13">
-        <f>SUM('Weekly Points'!F137:F151)+C11</f>
-        <v>228</v>
+        <f>SUMIFS('Weekly Points'!$F$2:$F$271,'Weekly Points'!$B$2:$B$271,"WHU-Tang-Clan",'Weekly Points'!$A$2:$A$271,B13)+C11</f>
+        <v>267</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -6269,8 +6269,8 @@
         <v>6</v>
       </c>
       <c r="C14">
-        <f>SUM('Weekly Points'!F152:F166)+C12</f>
-        <v>321</v>
+        <f>SUMIFS('Weekly Points'!$F$2:$F$271,'Weekly Points'!$B$2:$B$271,"Bazzers Ballers",'Weekly Points'!$A$2:$A$271,B14)+C12</f>
+        <v>392</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -6281,8 +6281,8 @@
         <v>6</v>
       </c>
       <c r="C15">
-        <f>SUM('Weekly Points'!F167:F181)+C13</f>
-        <v>263</v>
+        <f>SUMIFS('Weekly Points'!$F$2:$F$271,'Weekly Points'!$B$2:$B$271,"WHU-Tang-Clan",'Weekly Points'!$A$2:$A$271,B15)+C13</f>
+        <v>319</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -6293,8 +6293,8 @@
         <v>7</v>
       </c>
       <c r="C16">
-        <f>SUM('Weekly Points'!F182:F196)+C14</f>
-        <v>380</v>
+        <f>SUMIFS('Weekly Points'!$F$2:$F$271,'Weekly Points'!$B$2:$B$271,"Bazzers Ballers",'Weekly Points'!$A$2:$A$271,B16)+C14</f>
+        <v>428</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -6305,8 +6305,8 @@
         <v>7</v>
       </c>
       <c r="C17">
-        <f>SUM('Weekly Points'!F197:F211)+C15</f>
-        <v>307</v>
+        <f>SUMIFS('Weekly Points'!$F$2:$F$271,'Weekly Points'!$B$2:$B$271,"WHU-Tang-Clan",'Weekly Points'!$A$2:$A$271,B17)+C15</f>
+        <v>367</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -6317,8 +6317,8 @@
         <v>8</v>
       </c>
       <c r="C18">
-        <f>SUM('Weekly Points'!F212:F226)+C16</f>
-        <v>464</v>
+        <f>SUMIFS('Weekly Points'!$F$2:$F$271,'Weekly Points'!$B$2:$B$271,"Bazzers Ballers",'Weekly Points'!$A$2:$A$271,B18)+C16</f>
+        <v>456</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -6329,8 +6329,8 @@
         <v>8</v>
       </c>
       <c r="C19">
-        <f>SUM('Weekly Points'!F227:F241)+C17</f>
-        <v>376</v>
+        <f>SUMIFS('Weekly Points'!$F$2:$F$271,'Weekly Points'!$B$2:$B$271,"WHU-Tang-Clan",'Weekly Points'!$A$2:$A$271,B19)+C17</f>
+        <v>392</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -6341,7 +6341,7 @@
         <v>9</v>
       </c>
       <c r="C20">
-        <f>SUM('Weekly Points'!F242:F256)+C18</f>
+        <f>SUMIFS('Weekly Points'!$F$2:$F$271,'Weekly Points'!$B$2:$B$271,"Bazzers Ballers",'Weekly Points'!$A$2:$A$271,B20)+C18</f>
         <v>506</v>
       </c>
     </row>
@@ -6353,14 +6353,11 @@
         <v>9</v>
       </c>
       <c r="C21">
-        <f>SUM('Weekly Points'!F257:F271)+C19</f>
+        <f>SUMIFS('Weekly Points'!$F$2:$F$271,'Weekly Points'!$B$2:$B$271,"WHU-Tang-Clan",'Weekly Points'!$A$2:$A$271,B21)+C19</f>
         <v>439</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="C4:C5 C6 C7:C11 C12:C17 C18:C19 C20:C21" formulaRange="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Week 11 Updated (Amendment)
</commit_message>
<xml_diff>
--- a/WHUPUP.xlsx
+++ b/WHUPUP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28305"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\OneDrive\Desktop\F_Football\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ECADE78-4374-4C85-B1FF-165F58EAA8DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24246618-0B64-4D58-A0B6-EB051EB0E550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-60" windowWidth="23256" windowHeight="12576" xr2:uid="{99B477C4-CCE4-43A8-837E-CF46EFFB0705}"/>
+    <workbookView xWindow="22932" yWindow="-60" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{99B477C4-CCE4-43A8-837E-CF46EFFB0705}"/>
   </bookViews>
   <sheets>
     <sheet name="Weekly Points" sheetId="1" r:id="rId1"/>
@@ -659,7 +659,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDD6DB57-DBEF-439C-86C8-55613737F70F}">
   <dimension ref="A1:F331"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -7303,7 +7303,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4E08F3E-397A-4BD7-9E39-8A74D5B0AA3B}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
@@ -7595,8 +7595,8 @@
         <v>11</v>
       </c>
       <c r="C24">
-        <f>SUMIFS('Weekly Points'!$F$32:$F$361,'Weekly Points'!$B$32:$B$361,"Bazzers Ballers",'Weekly Points'!$A$32:$A$361,B24)+C22</f>
-        <v>530</v>
+        <f>SUMIFS('Weekly Points'!$F$2:$F$361,'Weekly Points'!$B$2:$B$361,"Bazzers Ballers",'Weekly Points'!$A$2:$A$361,B24)+C22</f>
+        <v>579</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -7607,8 +7607,8 @@
         <v>11</v>
       </c>
       <c r="C25">
-        <f>SUMIFS('Weekly Points'!$F$32:$F$361,'Weekly Points'!$B$32:$B$361,"WHU-Tang-Clan",'Weekly Points'!$A$32:$A$361,B25)+C23</f>
-        <v>465</v>
+        <f>SUMIFS('Weekly Points'!$F$2:$F$361,'Weekly Points'!$B$2:$B$361,"WHU-Tang-Clan",'Weekly Points'!$A$2:$A$361,B25)+C23</f>
+        <v>505</v>
       </c>
     </row>
   </sheetData>

</xml_diff>